<commit_message>
every 1 minute works
</commit_message>
<xml_diff>
--- a/MetaMarian_Robot/Data/Input/EmployeesInformations.xlsx
+++ b/MetaMarian_Robot/Data/Input/EmployeesInformations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosmin.oanea\Documents\IS\MetaMarian\MetaMarian_Robot\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CC5FC3-6CF9-44CB-807D-2A195CD5B5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532F5B14-EA7D-47F3-86F1-67BFF0FFAEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="151">
   <si>
     <t>First Name</t>
   </si>
@@ -481,6 +481,15 @@
   </si>
   <si>
     <t>cosminoanea01@gmail.com</t>
+  </si>
+  <si>
+    <t>employeetestproject@gmail.com</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Testescu</t>
   </si>
 </sst>
 </file>
@@ -862,7 +871,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1168,7 +1177,15 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D12" s="1"/>
+      <c r="A12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" s="1"/>

</xml_diff>

<commit_message>
Finished the task, added workflow for Codecademy
</commit_message>
<xml_diff>
--- a/MetaMarian_Robot/Data/Input/EmployeesInformations.xlsx
+++ b/MetaMarian_Robot/Data/Input/EmployeesInformations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosmin.oanea\Documents\IS\MetaMarian\MetaMarian_Robot\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\facultate\RPA\MetaMarian\MetaMarian_Robot\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532F5B14-EA7D-47F3-86F1-67BFF0FFAEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124300BC-1409-4B6F-8BBE-0B5230C1960B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,12 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -84,412 +78,412 @@
     <t>C,C++,Python</t>
   </si>
   <si>
+    <t>junior C++ developer</t>
+  </si>
+  <si>
+    <t>Andreea</t>
+  </si>
+  <si>
+    <t>Milu</t>
+  </si>
+  <si>
+    <t>Lalelelor Street,45,Cluj-Napoca,Romania,400049</t>
+  </si>
+  <si>
+    <t>andreea.milu@gmail.com</t>
+  </si>
+  <si>
+    <t>PHP,VB,C#,Python</t>
+  </si>
+  <si>
+    <t>business analysis</t>
+  </si>
+  <si>
+    <t>junior C# developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vlad </t>
+  </si>
+  <si>
+    <t>Lungu</t>
+  </si>
+  <si>
+    <t>Uverturii Boulevard,89,Bucharest,Romania,060936</t>
+  </si>
+  <si>
+    <t>vlad.lungu@gmail.com</t>
+  </si>
+  <si>
+    <t>C#,Java,Css,JavaScript</t>
+  </si>
+  <si>
+    <t>communication,marketing</t>
+  </si>
+  <si>
+    <t>full stack developer</t>
+  </si>
+  <si>
+    <t>Mihai</t>
+  </si>
+  <si>
+    <t>Obreja</t>
+  </si>
+  <si>
+    <t>Drumul Taberei Street,98,Bucharest,Romania,061409</t>
+  </si>
+  <si>
+    <t>mihai.obreja@gmail.com</t>
+  </si>
+  <si>
+    <t>ciprian.paduraru@gmail.com</t>
+  </si>
+  <si>
+    <t>Python,Java,VB</t>
+  </si>
+  <si>
+    <t>management,ui design</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>Cosmin</t>
+  </si>
+  <si>
+    <t>Popescu</t>
+  </si>
+  <si>
+    <t>Libertății Street,11,Pitești,Romania,110357</t>
+  </si>
+  <si>
+    <t>cosmin.popescu@gmail.com</t>
+  </si>
+  <si>
+    <t>C,C++,Python,Java</t>
+  </si>
+  <si>
+    <t>management,communication</t>
+  </si>
+  <si>
+    <t>junior Java developer</t>
+  </si>
+  <si>
+    <t>Valentina</t>
+  </si>
+  <si>
+    <t>Luță</t>
+  </si>
+  <si>
+    <t>Independenței Boulevard,5,Bistrița,Romania,420162</t>
+  </si>
+  <si>
+    <t>valentina.luta@gmail.com</t>
+  </si>
+  <si>
+    <t>mara.dascalu@gmail.com</t>
+  </si>
+  <si>
+    <t>PHP,TypeScript,JavaScript</t>
+  </si>
+  <si>
+    <t>graphic design,ux design</t>
+  </si>
+  <si>
+    <t>ui designer</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Ionescu</t>
+  </si>
+  <si>
+    <t>Regina Elisabeta Boulevard,42,Bucharest,Romania,050018</t>
+  </si>
+  <si>
+    <t>george.ionescu@gmail.com</t>
+  </si>
+  <si>
+    <t>C,Java,JavaScript,Css</t>
+  </si>
+  <si>
+    <t>ux design,ui design</t>
+  </si>
+  <si>
+    <t>ux designer</t>
+  </si>
+  <si>
+    <t>Ana-Maria</t>
+  </si>
+  <si>
+    <t>Firănescu</t>
+  </si>
+  <si>
+    <t>Dacia Boulevard,119,Craiova,Romania,200275</t>
+  </si>
+  <si>
+    <t>ana.firanescu@gmail.com</t>
+  </si>
+  <si>
+    <t>C,C++,Python,SQL</t>
+  </si>
+  <si>
+    <t>database manipulation</t>
+  </si>
+  <si>
+    <t>junior dbs</t>
+  </si>
+  <si>
+    <t>Ioan</t>
+  </si>
+  <si>
+    <t>Dorobanțu</t>
+  </si>
+  <si>
+    <t>Timișoara Boulevard,60,Bucharest,Romania,061333</t>
+  </si>
+  <si>
+    <t>ioan.dorobantu@gmail.com</t>
+  </si>
+  <si>
+    <t>mihaela.stanciu@gmail.com</t>
+  </si>
+  <si>
+    <t>C,Prolog,Haskell,Python,</t>
+  </si>
+  <si>
+    <t>devops,project management</t>
+  </si>
+  <si>
+    <t>devops</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Led department</t>
+  </si>
+  <si>
+    <t>Claudia</t>
+  </si>
+  <si>
+    <t>Crăciun</t>
+  </si>
+  <si>
+    <t>development department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mihaela </t>
+  </si>
+  <si>
+    <t>Stanciu</t>
+  </si>
+  <si>
+    <t>integration department</t>
+  </si>
+  <si>
+    <t>Ciprian</t>
+  </si>
+  <si>
+    <t>Păduraru</t>
+  </si>
+  <si>
+    <t>testing department</t>
+  </si>
+  <si>
+    <t>Mara Elena</t>
+  </si>
+  <si>
+    <t>Dascălu</t>
+  </si>
+  <si>
+    <t>the maintenance and technical support department</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>Alexandra</t>
+  </si>
+  <si>
+    <t>Badea</t>
+  </si>
+  <si>
+    <t>alexandra.badea@gmail.com</t>
+  </si>
+  <si>
+    <t>senior C++ developer</t>
+  </si>
+  <si>
+    <t>Catalin</t>
+  </si>
+  <si>
+    <t>Ilie</t>
+  </si>
+  <si>
+    <t>catalin.ilie@gmail.com</t>
+  </si>
+  <si>
+    <t>senior Java developer</t>
+  </si>
+  <si>
+    <t>Monica</t>
+  </si>
+  <si>
+    <t>Stamate</t>
+  </si>
+  <si>
+    <t>monica.stamate@gmail.com</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Crețu</t>
+  </si>
+  <si>
+    <t>maria.cretu@gmail.com</t>
+  </si>
+  <si>
+    <t>Claudiu</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>claudiu.pop@gmail.com</t>
+  </si>
+  <si>
+    <t>senior dba</t>
+  </si>
+  <si>
+    <t>Razvan</t>
+  </si>
+  <si>
+    <t>razvan.ionescu@gmail.com</t>
+  </si>
+  <si>
+    <t>Iulia</t>
+  </si>
+  <si>
+    <t>Grecu</t>
+  </si>
+  <si>
+    <t>iulia.grecu@gmail.com</t>
+  </si>
+  <si>
+    <t>Mihnea</t>
+  </si>
+  <si>
+    <t>Scurtu</t>
+  </si>
+  <si>
+    <t>mihnea.scurtu@gmail.com</t>
+  </si>
+  <si>
+    <t>project architect</t>
+  </si>
+  <si>
+    <t>Cristian</t>
+  </si>
+  <si>
+    <t>Cotoia</t>
+  </si>
+  <si>
+    <t>cristian.cotoia@gmail.com</t>
+  </si>
+  <si>
+    <t>senior C# developer</t>
+  </si>
+  <si>
+    <t>Marius</t>
+  </si>
+  <si>
+    <t>Goia</t>
+  </si>
+  <si>
+    <t>marius.goia@gmail.com</t>
+  </si>
+  <si>
+    <t>Andrei</t>
+  </si>
+  <si>
+    <t>Dumitrescu</t>
+  </si>
+  <si>
+    <t>andrei.dumitrescu@gmail.com</t>
+  </si>
+  <si>
+    <t>front end developer</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>https://clightning.medium.com/how-to-write-clean-beautiful-and-effective-c-code-d4699f5e3864</t>
+  </si>
+  <si>
+    <t>Clean code principles C++</t>
+  </si>
+  <si>
+    <t>https://userguiding.com/blog/ux-design-principles/</t>
+  </si>
+  <si>
+    <t>Fundamental UX Design Principles</t>
+  </si>
+  <si>
+    <t>https://support.microsoft.com/en-us/office/database-design-basics-eb2159cf-1e30-401a-8084-bd4f9c9ca1f5</t>
+  </si>
+  <si>
+    <t>Database design basics</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/JavaScript/Guide/Introduction#:~:text=JavaScript%20is%20a%20cross%2Dplatform,of%20JavaScript%20such%20as%20Node.</t>
+  </si>
+  <si>
+    <t>Introduction in JavaScript</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>Position in company</t>
+  </si>
+  <si>
+    <t>Number of hours of practice</t>
+  </si>
+  <si>
+    <t>Tudor Cosmin</t>
+  </si>
+  <si>
+    <t>Oanea</t>
+  </si>
+  <si>
+    <t>grozavesti</t>
+  </si>
+  <si>
+    <t>cosminoanea01@gmail.com</t>
+  </si>
+  <si>
+    <t>employeetestproject@gmail.com</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Testescu</t>
+  </si>
+  <si>
     <t>graphic design,marketing</t>
-  </si>
-  <si>
-    <t>junior C++ developer</t>
-  </si>
-  <si>
-    <t>Andreea</t>
-  </si>
-  <si>
-    <t>Milu</t>
-  </si>
-  <si>
-    <t>Lalelelor Street,45,Cluj-Napoca,Romania,400049</t>
-  </si>
-  <si>
-    <t>andreea.milu@gmail.com</t>
-  </si>
-  <si>
-    <t>PHP,VB,C#,Python</t>
-  </si>
-  <si>
-    <t>business analysis</t>
-  </si>
-  <si>
-    <t>junior C# developer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vlad </t>
-  </si>
-  <si>
-    <t>Lungu</t>
-  </si>
-  <si>
-    <t>Uverturii Boulevard,89,Bucharest,Romania,060936</t>
-  </si>
-  <si>
-    <t>vlad.lungu@gmail.com</t>
-  </si>
-  <si>
-    <t>C#,Java,Css,JavaScript</t>
-  </si>
-  <si>
-    <t>communication,marketing</t>
-  </si>
-  <si>
-    <t>full stack developer</t>
-  </si>
-  <si>
-    <t>Mihai</t>
-  </si>
-  <si>
-    <t>Obreja</t>
-  </si>
-  <si>
-    <t>Drumul Taberei Street,98,Bucharest,Romania,061409</t>
-  </si>
-  <si>
-    <t>mihai.obreja@gmail.com</t>
-  </si>
-  <si>
-    <t>ciprian.paduraru@gmail.com</t>
-  </si>
-  <si>
-    <t>Python,Java,VB</t>
-  </si>
-  <si>
-    <t>management,ui design</t>
-  </si>
-  <si>
-    <t>tester</t>
-  </si>
-  <si>
-    <t>Cosmin</t>
-  </si>
-  <si>
-    <t>Popescu</t>
-  </si>
-  <si>
-    <t>Libertății Street,11,Pitești,Romania,110357</t>
-  </si>
-  <si>
-    <t>cosmin.popescu@gmail.com</t>
-  </si>
-  <si>
-    <t>C,C++,Python,Java</t>
-  </si>
-  <si>
-    <t>management,communication</t>
-  </si>
-  <si>
-    <t>junior Java developer</t>
-  </si>
-  <si>
-    <t>Valentina</t>
-  </si>
-  <si>
-    <t>Luță</t>
-  </si>
-  <si>
-    <t>Independenței Boulevard,5,Bistrița,Romania,420162</t>
-  </si>
-  <si>
-    <t>valentina.luta@gmail.com</t>
-  </si>
-  <si>
-    <t>mara.dascalu@gmail.com</t>
-  </si>
-  <si>
-    <t>PHP,TypeScript,JavaScript</t>
-  </si>
-  <si>
-    <t>graphic design,ux design</t>
-  </si>
-  <si>
-    <t>ui designer</t>
-  </si>
-  <si>
-    <t>George</t>
-  </si>
-  <si>
-    <t>Ionescu</t>
-  </si>
-  <si>
-    <t>Regina Elisabeta Boulevard,42,Bucharest,Romania,050018</t>
-  </si>
-  <si>
-    <t>george.ionescu@gmail.com</t>
-  </si>
-  <si>
-    <t>C,Java,JavaScript,Css</t>
-  </si>
-  <si>
-    <t>ux design,ui design</t>
-  </si>
-  <si>
-    <t>ux designer</t>
-  </si>
-  <si>
-    <t>Ana-Maria</t>
-  </si>
-  <si>
-    <t>Firănescu</t>
-  </si>
-  <si>
-    <t>Dacia Boulevard,119,Craiova,Romania,200275</t>
-  </si>
-  <si>
-    <t>ana.firanescu@gmail.com</t>
-  </si>
-  <si>
-    <t>C,C++,Python,SQL</t>
-  </si>
-  <si>
-    <t>database manipulation</t>
-  </si>
-  <si>
-    <t>junior dbs</t>
-  </si>
-  <si>
-    <t>Ioan</t>
-  </si>
-  <si>
-    <t>Dorobanțu</t>
-  </si>
-  <si>
-    <t>Timișoara Boulevard,60,Bucharest,Romania,061333</t>
-  </si>
-  <si>
-    <t>ioan.dorobantu@gmail.com</t>
-  </si>
-  <si>
-    <t>mihaela.stanciu@gmail.com</t>
-  </si>
-  <si>
-    <t>C,Prolog,Haskell,Python,</t>
-  </si>
-  <si>
-    <t>devops,project management</t>
-  </si>
-  <si>
-    <t>devops</t>
-  </si>
-  <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
-    <t>Led department</t>
-  </si>
-  <si>
-    <t>Claudia</t>
-  </si>
-  <si>
-    <t>Crăciun</t>
-  </si>
-  <si>
-    <t>development department</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mihaela </t>
-  </si>
-  <si>
-    <t>Stanciu</t>
-  </si>
-  <si>
-    <t>integration department</t>
-  </si>
-  <si>
-    <t>Ciprian</t>
-  </si>
-  <si>
-    <t>Păduraru</t>
-  </si>
-  <si>
-    <t>testing department</t>
-  </si>
-  <si>
-    <t>Mara Elena</t>
-  </si>
-  <si>
-    <t>Dascălu</t>
-  </si>
-  <si>
-    <t>the maintenance and technical support department</t>
-  </si>
-  <si>
-    <t>Availability</t>
-  </si>
-  <si>
-    <t>Alexandra</t>
-  </si>
-  <si>
-    <t>Badea</t>
-  </si>
-  <si>
-    <t>alexandra.badea@gmail.com</t>
-  </si>
-  <si>
-    <t>senior C++ developer</t>
-  </si>
-  <si>
-    <t>Catalin</t>
-  </si>
-  <si>
-    <t>Ilie</t>
-  </si>
-  <si>
-    <t>catalin.ilie@gmail.com</t>
-  </si>
-  <si>
-    <t>senior Java developer</t>
-  </si>
-  <si>
-    <t>Monica</t>
-  </si>
-  <si>
-    <t>Stamate</t>
-  </si>
-  <si>
-    <t>monica.stamate@gmail.com</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Crețu</t>
-  </si>
-  <si>
-    <t>maria.cretu@gmail.com</t>
-  </si>
-  <si>
-    <t>Claudiu</t>
-  </si>
-  <si>
-    <t>Pop</t>
-  </si>
-  <si>
-    <t>claudiu.pop@gmail.com</t>
-  </si>
-  <si>
-    <t>senior dba</t>
-  </si>
-  <si>
-    <t>Razvan</t>
-  </si>
-  <si>
-    <t>razvan.ionescu@gmail.com</t>
-  </si>
-  <si>
-    <t>Iulia</t>
-  </si>
-  <si>
-    <t>Grecu</t>
-  </si>
-  <si>
-    <t>iulia.grecu@gmail.com</t>
-  </si>
-  <si>
-    <t>Mihnea</t>
-  </si>
-  <si>
-    <t>Scurtu</t>
-  </si>
-  <si>
-    <t>mihnea.scurtu@gmail.com</t>
-  </si>
-  <si>
-    <t>project architect</t>
-  </si>
-  <si>
-    <t>Cristian</t>
-  </si>
-  <si>
-    <t>Cotoia</t>
-  </si>
-  <si>
-    <t>cristian.cotoia@gmail.com</t>
-  </si>
-  <si>
-    <t>senior C# developer</t>
-  </si>
-  <si>
-    <t>Marius</t>
-  </si>
-  <si>
-    <t>Goia</t>
-  </si>
-  <si>
-    <t>marius.goia@gmail.com</t>
-  </si>
-  <si>
-    <t>Andrei</t>
-  </si>
-  <si>
-    <t>Dumitrescu</t>
-  </si>
-  <si>
-    <t>andrei.dumitrescu@gmail.com</t>
-  </si>
-  <si>
-    <t>front end developer</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>https://clightning.medium.com/how-to-write-clean-beautiful-and-effective-c-code-d4699f5e3864</t>
-  </si>
-  <si>
-    <t>Clean code principles C++</t>
-  </si>
-  <si>
-    <t>https://userguiding.com/blog/ux-design-principles/</t>
-  </si>
-  <si>
-    <t>Fundamental UX Design Principles</t>
-  </si>
-  <si>
-    <t>https://support.microsoft.com/en-us/office/database-design-basics-eb2159cf-1e30-401a-8084-bd4f9c9ca1f5</t>
-  </si>
-  <si>
-    <t>Database design basics</t>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/en-US/docs/Web/JavaScript/Guide/Introduction#:~:text=JavaScript%20is%20a%20cross%2Dplatform,of%20JavaScript%20such%20as%20Node.</t>
-  </si>
-  <si>
-    <t>Introduction in JavaScript</t>
-  </si>
-  <si>
-    <t>Faculty</t>
-  </si>
-  <si>
-    <t>University</t>
-  </si>
-  <si>
-    <t>Position in company</t>
-  </si>
-  <si>
-    <t>Number of hours of practice</t>
-  </si>
-  <si>
-    <t>Tudor Cosmin</t>
-  </si>
-  <si>
-    <t>Oanea</t>
-  </si>
-  <si>
-    <t>grozavesti</t>
-  </si>
-  <si>
-    <t>cosminoanea01@gmail.com</t>
-  </si>
-  <si>
-    <t>employeetestproject@gmail.com</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Testescu</t>
   </si>
 </sst>
 </file>
@@ -870,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -936,255 +930,255 @@
         <v>14</v>
       </c>
       <c r="H2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" t="s">
         <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" t="s">
         <v>35</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>36</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>37</v>
-      </c>
-      <c r="I5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
         <v>43</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>44</v>
-      </c>
-      <c r="I6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
         <v>46</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" t="s">
         <v>50</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>52</v>
-      </c>
-      <c r="I7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>58</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>59</v>
-      </c>
-      <c r="I8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
         <v>61</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>62</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>65</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>66</v>
-      </c>
-      <c r="I9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
         <v>68</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>69</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" t="s">
         <v>72</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>73</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>74</v>
-      </c>
-      <c r="I10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" t="s">
         <v>144</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>145</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="F11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" t="s">
         <v>72</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>73</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>74</v>
-      </c>
-      <c r="I11" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" t="s">
         <v>149</v>
       </c>
-      <c r="B12" t="s">
-        <v>150</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1265,72 +1259,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
-      </c>
-      <c r="B1" t="s">
-        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
         <v>79</v>
-      </c>
-      <c r="B2" t="s">
-        <v>80</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
         <v>85</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
         <v>86</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1364,10 +1358,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
-      </c>
-      <c r="B1" t="s">
-        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1376,171 +1370,171 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
         <v>92</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" t="s">
         <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>95</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
         <v>96</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
         <v>98</v>
-      </c>
-      <c r="D3" t="s">
-        <v>99</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
         <v>100</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
         <v>103</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
         <v>106</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" t="s">
         <v>108</v>
-      </c>
-      <c r="D6" t="s">
-        <v>109</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
         <v>112</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="s">
         <v>115</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" t="s">
         <v>117</v>
-      </c>
-      <c r="D9" t="s">
-        <v>118</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" t="s">
         <v>119</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" t="s">
         <v>121</v>
-      </c>
-      <c r="D10" t="s">
-        <v>122</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" t="s">
         <v>123</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
         <v>126</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" t="s">
         <v>128</v>
-      </c>
-      <c r="D12" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1577,42 +1571,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
         <v>130</v>
-      </c>
-      <c r="B1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
         <v>132</v>
-      </c>
-      <c r="B2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
         <v>134</v>
-      </c>
-      <c r="B3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" t="s">
         <v>136</v>
-      </c>
-      <c r="B4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" t="s">
         <v>138</v>
-      </c>
-      <c r="B5" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1647,25 +1641,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
-      </c>
-      <c r="B1" t="s">
-        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" t="s">
         <v>140</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>141</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>142</v>
-      </c>
-      <c r="G1" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the excel test file
</commit_message>
<xml_diff>
--- a/MetaMarian_Robot/Data/Input/EmployeesInformations.xlsx
+++ b/MetaMarian_Robot/Data/Input/EmployeesInformations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosmin.oanea\Documents\IS\MetaMarian\MetaMarian_Robot\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532F5B14-EA7D-47F3-86F1-67BFF0FFAEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{280C8D28-7AC5-4190-909C-6434084377D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="152">
   <si>
     <t>First Name</t>
   </si>
@@ -267,6 +267,27 @@
     <t>devops</t>
   </si>
   <si>
+    <t>Tudor Cosmin</t>
+  </si>
+  <si>
+    <t>Oanea</t>
+  </si>
+  <si>
+    <t>grozavesti</t>
+  </si>
+  <si>
+    <t>cosminoanea01@gmail.com</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Testescu</t>
+  </si>
+  <si>
+    <t>employeetestproject@gmail.com</t>
+  </si>
+  <si>
     <t>First name</t>
   </si>
   <si>
@@ -327,6 +348,9 @@
     <t>senior C++ developer</t>
   </si>
   <si>
+    <t>YES</t>
+  </si>
+  <si>
     <t>Catalin</t>
   </si>
   <si>
@@ -469,34 +493,13 @@
   </si>
   <si>
     <t>Number of hours of practice</t>
-  </si>
-  <si>
-    <t>Tudor Cosmin</t>
-  </si>
-  <si>
-    <t>Oanea</t>
-  </si>
-  <si>
-    <t>grozavesti</t>
-  </si>
-  <si>
-    <t>cosminoanea01@gmail.com</t>
-  </si>
-  <si>
-    <t>employeetestproject@gmail.com</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Testescu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,6 +526,13 @@
       <color rgb="FF24292F"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -545,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -553,6 +563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -572,7 +583,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -860,7 +871,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -870,24 +881,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" customWidth="1"/>
-    <col min="2" max="2" width="34.7265625" customWidth="1"/>
-    <col min="3" max="3" width="50.81640625" customWidth="1"/>
-    <col min="4" max="4" width="30.453125" customWidth="1"/>
-    <col min="5" max="5" width="33.453125" customWidth="1"/>
-    <col min="6" max="6" width="28.54296875" customWidth="1"/>
-    <col min="7" max="7" width="37.453125" customWidth="1"/>
-    <col min="8" max="8" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
+    <col min="7" max="7" width="37.42578125" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -916,7 +927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -942,7 +953,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -968,7 +979,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -994,7 +1005,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1020,7 +1031,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1046,7 +1057,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1072,7 +1083,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1098,7 +1109,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -1124,7 +1135,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -1150,18 +1161,18 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>147</v>
+        <v>79</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>72</v>
@@ -1176,48 +1187,48 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>81</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4">
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4">
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4">
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4">
       <c r="D23" s="1"/>
     </row>
   </sheetData>
@@ -1255,82 +1266,82 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="46.26953125" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1348,26 +1359,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC2AAA9F-384C-463A-8EE0-84D713D4D9FD}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
-    <col min="3" max="3" width="28.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" customWidth="1"/>
-    <col min="8" max="8" width="28.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1376,171 +1387,194 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D8" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D11" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>137</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1569,50 +1603,50 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="117" customWidth="1"/>
-    <col min="2" max="2" width="48.81640625" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1634,38 +1668,38 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" customWidth="1"/>
-    <col min="6" max="6" width="24.453125" customWidth="1"/>
-    <col min="7" max="7" width="24.7265625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="E1" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="F1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="G1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>